<commit_message>
Bot level 2 full
</commit_message>
<xml_diff>
--- a/1. Documentos_ xml_xlsx/from.xlsx
+++ b/1. Documentos_ xml_xlsx/from.xlsx
@@ -1,107 +1,88 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\yolima alejandra\desktop\robots\1. documentos_ xml_xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yolima Alejandra\Desktop\Robots\1. Documentos_ xml_xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1BF9FA7-1800-4F66-896F-4A972EC8293B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A33875C-8CF3-4501-BFF7-CD2DA9808325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2850" yWindow="2850" windowWidth="15375" windowHeight="7875" xr2:uid="{F8260453-F432-41DE-B9F8-5256DF080983}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
-<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{07C472CF-5822-4556-94E0-54CC46DCB1CA}" name="datos" type="4" refreshedVersion="0" background="1">
-    <webPr xml="1" sourceData="1" url="C:\Users\Yolima Alejandra\Desktop\2botFinal\datos.xml" htmlTables="1" htmlFormat="all"/>
-  </connection>
-</connections>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Message</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>assist</t>
-  </si>
-  <si>
-    <t>Alejandra</t>
-  </si>
-  <si>
-    <t>aleja@gmail.com</t>
-  </si>
-  <si>
-    <t>Colombia</t>
-  </si>
-  <si>
-    <t>revisar bot</t>
-  </si>
-  <si>
-    <t>udemy</t>
-  </si>
-  <si>
-    <t>Mary</t>
-  </si>
-  <si>
-    <t>mar@gmail.com</t>
-  </si>
-  <si>
-    <t>Chile</t>
-  </si>
-  <si>
-    <t>curso rocketbot finalizado</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+  <si>
+    <t>Id_Producto</t>
+  </si>
+  <si>
+    <t>Codigo</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Medida</t>
+  </si>
+  <si>
+    <t>Costo_Compra</t>
+  </si>
+  <si>
+    <t>Costo_venta</t>
+  </si>
+  <si>
+    <t>P006</t>
+  </si>
+  <si>
+    <t>Hojas Bond</t>
+  </si>
+  <si>
+    <t>Ciento</t>
+  </si>
+  <si>
+    <t>P007</t>
+  </si>
+  <si>
+    <t>Cuaderno Universitario</t>
+  </si>
+  <si>
+    <t>P008</t>
+  </si>
+  <si>
+    <t>Papel iris</t>
+  </si>
+  <si>
+    <t>P009</t>
+  </si>
+  <si>
+    <t>Carton cartulina</t>
+  </si>
+  <si>
+    <t>P010</t>
+  </si>
+  <si>
+    <t>Papeleria de regalo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,28 +93,6 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -157,26 +116,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -190,71 +137,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
-<MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
-  <Schema ID="Schema1">
-    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
-      <xsd:element nillable="true" name="FT009">
-        <xsd:complexType>
-          <xsd:sequence minOccurs="0">
-            <xsd:element minOccurs="0" nillable="true" name="RegistroFT009" form="unqualified">
-              <xsd:complexType>
-                <xsd:sequence minOccurs="0">
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="company" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="name" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="email" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="phone" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="country" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="message" form="unqualified"/>
-                </xsd:sequence>
-              </xsd:complexType>
-            </xsd:element>
-          </xsd:sequence>
-        </xsd:complexType>
-      </xsd:element>
-    </xsd:schema>
-  </Schema>
-  <Map ID="1" Name="FT009_Map" RootElement="FT009" SchemaID="Schema1" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="1" DataBindingLoadMode="1"/>
-  </Map>
-</MapInfo>
-</file>
-
-<file path=xl/tables/tableSingleCells1.xml><?xml version="1.0" encoding="utf-8"?>
-<singleXmlCells xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="xr xr3 xr6">
-  <singleXmlCell id="1" xr6:uid="{92819758-697A-4E6C-9FD7-16C7A471AD4F}" r="A1" connectionId="1">
-    <xmlCellPr id="1" xr6:uid="{DD84495E-A687-4295-AEE6-9D82DE2FE80D}" uniqueName="company">
-      <xmlPr mapId="1" xpath="/FT009/RegistroFT009/company" xmlDataType="string"/>
-    </xmlCellPr>
-  </singleXmlCell>
-  <singleXmlCell id="2" xr6:uid="{EDCDAAB3-E1A9-4D53-A186-0AF9C0E13EC2}" r="B1" connectionId="1">
-    <xmlCellPr id="1" xr6:uid="{01365BD1-3739-4937-B724-2D4193E6A8C4}" uniqueName="name">
-      <xmlPr mapId="1" xpath="/FT009/RegistroFT009/name" xmlDataType="string"/>
-    </xmlCellPr>
-  </singleXmlCell>
-  <singleXmlCell id="3" xr6:uid="{A510BBD3-B934-4596-A65B-D6A3DB8AEF20}" r="C1" connectionId="1">
-    <xmlCellPr id="1" xr6:uid="{571EE975-47D4-492E-A42D-DFBF018B9707}" uniqueName="email">
-      <xmlPr mapId="1" xpath="/FT009/RegistroFT009/email" xmlDataType="string"/>
-    </xmlCellPr>
-  </singleXmlCell>
-  <singleXmlCell id="4" xr6:uid="{D3B8C086-BF6C-48FE-82F5-9D0A6D485FC9}" r="D1" connectionId="1">
-    <xmlCellPr id="1" xr6:uid="{C4B8E674-5D43-4192-A265-4B47D4175C85}" uniqueName="phone">
-      <xmlPr mapId="1" xpath="/FT009/RegistroFT009/phone" xmlDataType="string"/>
-    </xmlCellPr>
-  </singleXmlCell>
-  <singleXmlCell id="5" xr6:uid="{77C69B92-7BB6-4D82-8A64-93326C0B9683}" r="E1" connectionId="1">
-    <xmlCellPr id="1" xr6:uid="{26DB3824-E300-4D59-AEC9-25B6AADCDF40}" uniqueName="country">
-      <xmlPr mapId="1" xpath="/FT009/RegistroFT009/country" xmlDataType="string"/>
-    </xmlCellPr>
-  </singleXmlCell>
-  <singleXmlCell id="6" xr6:uid="{7B5D8CC3-5BD3-4C10-B51E-0D78B91D697F}" r="F1" connectionId="1">
-    <xmlCellPr id="1" xr6:uid="{E7AB634A-B31A-4FB2-ADAA-0584E65842C3}" uniqueName="message">
-      <xmlPr mapId="1" xpath="/FT009/RegistroFT009/message" xmlDataType="string"/>
-    </xmlCellPr>
-  </singleXmlCell>
-</singleXmlCells>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -274,7 +156,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -286,7 +168,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -333,23 +215,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -385,23 +250,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -553,84 +401,141 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4AE139-6B82-437A-BBC8-71648A0265F1}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="A2:G2"/>
+      <selection activeCell="G8" sqref="A2:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>120000</v>
+      </c>
+      <c r="F2">
+        <v>150000</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2">
-        <v>3177378803</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="E3">
+        <v>200000</v>
+      </c>
+      <c r="F3">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>189000</v>
+      </c>
+      <c r="F4">
+        <v>215000</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="39" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2">
-        <v>3022828282</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>90000</v>
+      </c>
+      <c r="F5">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="C6" t="s">
         <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>80000</v>
+      </c>
+      <c r="F6">
+        <v>100000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>